<commit_message>
testdatanew.xlsx is updated and two other files were changed
</commit_message>
<xml_diff>
--- a/testdatanew.xlsx
+++ b/testdatanew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkar\source\repos\TestingEG\TestingEG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8E4004-CF01-49E4-A36E-13C3E02CD5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7187079E-B3B5-4D8B-95B6-2BE650BC044A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Shravya1</t>
+  </si>
+  <si>
+    <t>Shravya2</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,6 +389,14 @@
         <v>2345</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>